<commit_message>
added 1.5h of work for correction
</commit_message>
<xml_diff>
--- a/Recherche/appendix/ILV.xlsx
+++ b/Recherche/appendix/ILV.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ramiro18/Library/Group Containers/UBF8T346G9.ms/MerpTempItems/Schule/Studium/Pro1/Recherche/appendix/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frank/Pro1/Recherche/appendix/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{231F41EE-8D7E-8A40-9E9D-698276C3B6EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2DBBA8-FD2B-A140-8921-601E03AAA9F1}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="8200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4320" yWindow="3300" windowWidth="16380" windowHeight="8200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recherche-Dokument" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
   <si>
     <t>ILV</t>
   </si>
@@ -94,9 +94,6 @@
   </si>
   <si>
     <t>Protokolle1&amp;2 erstellt + geschrieben                  Recherche</t>
-  </si>
-  <si>
-    <t>3,5</t>
   </si>
   <si>
     <t xml:space="preserve">Protokoll 2 angepasst                                                  zusätzliche Änderung                                                        Vorlage Einladung                                                                         </t>
@@ -505,7 +502,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -589,7 +586,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -887,8 +884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C9" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -964,11 +961,11 @@
       <c r="D10" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="14">
+        <v>5</v>
+      </c>
+      <c r="F10" s="15" t="s">
         <v>20</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="48" x14ac:dyDescent="0.2">

</xml_diff>